<commit_message>
Username Change in Config File
</commit_message>
<xml_diff>
--- a/G400_Automation/Resources/Config.xlsx
+++ b/G400_Automation/Resources/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER-L038\Desktop\Project\G400_Automation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER-L038\Desktop\Project\G400_Automation\G400_Automation_1\G400_Automation\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E36CFC26-C4E8-40C3-9AE5-DC8363A6A0EA}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73AA1526-4596-4326-833C-67278008F364}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{D200206D-3156-4F4D-9559-EFD096B95577}"/>
   </bookViews>
@@ -37,9 +37,6 @@
     <t>Password</t>
   </si>
   <si>
-    <t>HKSYN04</t>
-  </si>
-  <si>
     <t>complex1</t>
   </si>
   <si>
@@ -176,6 +173,9 @@
   </si>
   <si>
     <t>Policy_No</t>
+  </si>
+  <si>
+    <t>HKSYN03</t>
   </si>
 </sst>
 </file>
@@ -605,7 +605,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -624,10 +624,10 @@
     </row>
     <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -656,30 +656,30 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C2" s="2">
         <v>6</v>
@@ -691,15 +691,15 @@
         <v>2</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C3" s="2">
         <v>12</v>
@@ -711,15 +711,15 @@
         <v>20</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C4" s="2">
         <v>12</v>
@@ -731,15 +731,15 @@
         <v>20</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C5" s="2">
         <v>10</v>
@@ -751,15 +751,15 @@
         <v>2</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C6" s="2">
         <v>9</v>
@@ -771,15 +771,15 @@
         <v>3</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C7" s="2">
         <v>3</v>
@@ -791,15 +791,15 @@
         <v>2</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C8" s="2">
         <v>7</v>
@@ -811,15 +811,15 @@
         <v>10</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C9" s="2">
         <v>17</v>
@@ -831,15 +831,15 @@
         <v>1</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C10" s="2">
         <v>15</v>
@@ -851,15 +851,15 @@
         <v>10</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C11" s="2">
         <v>4</v>
@@ -871,15 +871,15 @@
         <v>20</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C12" s="2">
         <v>2</v>
@@ -891,15 +891,15 @@
         <v>15</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C13" s="2">
         <v>14</v>
@@ -911,15 +911,15 @@
         <v>7</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C14" s="2">
         <v>14</v>
@@ -931,15 +931,15 @@
         <v>15</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C15" s="2">
         <v>17</v>
@@ -951,15 +951,15 @@
         <v>8</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C16" s="2">
         <v>6</v>
@@ -971,15 +971,15 @@
         <v>10</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C17" s="2">
         <v>12</v>
@@ -991,15 +991,15 @@
         <v>1</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C18" s="2">
         <v>12</v>
@@ -1011,15 +1011,15 @@
         <v>10</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C19" s="2">
         <v>12</v>
@@ -1031,7 +1031,7 @@
         <v>3</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1059,26 +1059,26 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>26</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -1105,30 +1105,30 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>35</v>
-      </c>
       <c r="C1" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D2" s="2">
         <v>14</v>
@@ -1160,24 +1160,24 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>35</v>
-      </c>
       <c r="C1" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>38</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C2" s="2">
         <v>8</v>
@@ -1188,10 +1188,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>41</v>
       </c>
       <c r="C3" s="2">
         <v>8</v>

</xml_diff>